<commit_message>
add G: to schedule
</commit_message>
<xml_diff>
--- a/Copy of 08-04-24 to 08-10-24 Milwaukee Schedule Copy.xlsx
+++ b/Copy of 08-04-24 to 08-10-24 Milwaukee Schedule Copy.xlsx
@@ -635,7 +635,7 @@
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
         <is>
-          <t>G: 5:15 AM MEET GRAFTON PARK N RIDE</t>
+          <t>G: 5:00 AM MEET GRAFTON PARK N RIDE</t>
         </is>
       </c>
       <c r="S7" t="inlineStr"/>
@@ -2626,7 +2626,7 @@
       <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
-          <t>M: 4:30 AM MEET AT BAYSHORE
+          <t>M: 4:30 AM MEET AT BAYSHORE +
 G: 4:50 AM MEET GRAFTON PARK N RIDE</t>
         </is>
       </c>

</xml_diff>